<commit_message>
Updating Game Level Design and files
Updating the Game Level Designs
-nodes loaded into the server
-everything display correctly on the scene
</commit_message>
<xml_diff>
--- a/Game Level Designs.xlsx
+++ b/Game Level Designs.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7419151-5AC0-4163-8DBB-D37A5AFDD457}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16EAD4E-863F-42C1-8614-D51CB17D69B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645" tabRatio="749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645" tabRatio="749" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Level 1" sheetId="3" r:id="rId1"/>
     <sheet name="Game Level" sheetId="8" r:id="rId2"/>
     <sheet name="Game Level(Nodes)" sheetId="7" r:id="rId3"/>
-    <sheet name="New Mega Level" sheetId="6" state="hidden" r:id="rId4"/>
-    <sheet name="New Mega Level(Nodes)" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Game Level(Blocks)" sheetId="9" r:id="rId4"/>
+    <sheet name="New Mega Level" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="New Mega Level(Nodes)" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>n</t>
   </si>
@@ -126,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +169,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -639,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -814,6 +822,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,48 +1211,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="66"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="86"/>
     </row>
     <row r="2" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="69"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="89"/>
     </row>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -1208,10 +1276,10 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="W3" s="70" t="s">
+      <c r="W3" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="70"/>
+      <c r="X3" s="90"/>
     </row>
     <row r="4" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="21"/>
@@ -1700,56 +1768,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="66"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="86"/>
     </row>
     <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="69"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -1900,10 +1968,10 @@
       <c r="X6" s="2">
         <v>9</v>
       </c>
-      <c r="Z6" s="71" t="s">
+      <c r="Z6" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="72"/>
+      <c r="AA6" s="92"/>
     </row>
     <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
@@ -2569,8 +2637,8 @@
   </sheetPr>
   <dimension ref="B1:AA27"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView showFormulas="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,56 +2667,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="66"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="86"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="69"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -2813,10 +2881,10 @@
       <c r="X6" s="2">
         <v>9</v>
       </c>
-      <c r="Z6" s="70" t="s">
+      <c r="Z6" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="70"/>
+      <c r="AA6" s="90"/>
     </row>
     <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
@@ -3714,6 +3782,1231 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953A947D-DDD1-437C-AD35-EC677DFDDFDA}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B1:AA27"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" customWidth="1"/>
+    <col min="26" max="26" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B1" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="86"/>
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89"/>
+    </row>
+    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21"/>
+      <c r="C4" s="7">
+        <v>-10</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-9</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-8</v>
+      </c>
+      <c r="F4" s="7">
+        <v>-7</v>
+      </c>
+      <c r="G4" s="7">
+        <v>-6</v>
+      </c>
+      <c r="H4" s="7">
+        <v>-5</v>
+      </c>
+      <c r="I4" s="7">
+        <v>-4</v>
+      </c>
+      <c r="J4" s="7">
+        <v>-3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>-2</v>
+      </c>
+      <c r="L4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1</v>
+      </c>
+      <c r="O4" s="7">
+        <v>2</v>
+      </c>
+      <c r="P4" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>4</v>
+      </c>
+      <c r="R4" s="7">
+        <v>5</v>
+      </c>
+      <c r="S4" s="7">
+        <v>6</v>
+      </c>
+      <c r="T4" s="7">
+        <v>7</v>
+      </c>
+      <c r="U4" s="7">
+        <v>8</v>
+      </c>
+      <c r="V4" s="7">
+        <v>9</v>
+      </c>
+      <c r="W4" s="7">
+        <v>10</v>
+      </c>
+      <c r="X4" s="20"/>
+    </row>
+    <row r="5" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="66">
+        <v>0</v>
+      </c>
+      <c r="K5" s="64"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="64"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>9</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="66">
+        <v>1</v>
+      </c>
+      <c r="E6" s="66">
+        <v>2</v>
+      </c>
+      <c r="F6" s="65"/>
+      <c r="G6" s="66">
+        <v>3</v>
+      </c>
+      <c r="H6" s="66">
+        <v>4</v>
+      </c>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66">
+        <v>5</v>
+      </c>
+      <c r="K6" s="65"/>
+      <c r="L6" s="66">
+        <v>6</v>
+      </c>
+      <c r="M6" s="66">
+        <v>7</v>
+      </c>
+      <c r="N6" s="66">
+        <v>8</v>
+      </c>
+      <c r="O6" s="65"/>
+      <c r="P6" s="66">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="66">
+        <v>10</v>
+      </c>
+      <c r="R6" s="66">
+        <v>11</v>
+      </c>
+      <c r="S6" s="65"/>
+      <c r="T6" s="66">
+        <v>12</v>
+      </c>
+      <c r="U6" s="66">
+        <v>13</v>
+      </c>
+      <c r="V6" s="66">
+        <v>14</v>
+      </c>
+      <c r="W6" s="65"/>
+      <c r="X6" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="90"/>
+    </row>
+    <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66">
+        <v>15</v>
+      </c>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="66">
+        <v>16</v>
+      </c>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="66">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="67">
+        <v>159</v>
+      </c>
+      <c r="R7" s="66">
+        <v>18</v>
+      </c>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="66">
+        <v>19</v>
+      </c>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="2">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66">
+        <v>20</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="66">
+        <v>21</v>
+      </c>
+      <c r="G8" s="66">
+        <v>22</v>
+      </c>
+      <c r="H8" s="65"/>
+      <c r="I8" s="66">
+        <v>23</v>
+      </c>
+      <c r="J8" s="65"/>
+      <c r="K8" s="66">
+        <v>24</v>
+      </c>
+      <c r="L8" s="64"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="66">
+        <v>25</v>
+      </c>
+      <c r="P8" s="66">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="66">
+        <v>27</v>
+      </c>
+      <c r="S8" s="66">
+        <v>28</v>
+      </c>
+      <c r="T8" s="64"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="66">
+        <v>29</v>
+      </c>
+      <c r="X8" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="66">
+        <v>30</v>
+      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="66">
+        <v>31</v>
+      </c>
+      <c r="N9" s="64"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="66">
+        <v>32</v>
+      </c>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="66">
+        <v>33</v>
+      </c>
+      <c r="D10" s="66">
+        <v>34</v>
+      </c>
+      <c r="E10" s="66">
+        <v>35</v>
+      </c>
+      <c r="F10" s="65"/>
+      <c r="G10" s="66">
+        <v>36</v>
+      </c>
+      <c r="H10" s="66">
+        <v>37</v>
+      </c>
+      <c r="I10" s="66">
+        <v>38</v>
+      </c>
+      <c r="J10" s="65"/>
+      <c r="K10" s="66">
+        <v>39</v>
+      </c>
+      <c r="L10" s="65"/>
+      <c r="M10" s="66">
+        <v>40</v>
+      </c>
+      <c r="N10" s="65"/>
+      <c r="O10" s="66">
+        <v>41</v>
+      </c>
+      <c r="P10" s="66">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="66">
+        <v>43</v>
+      </c>
+      <c r="R10" s="66">
+        <v>44</v>
+      </c>
+      <c r="S10" s="66">
+        <v>45</v>
+      </c>
+      <c r="T10" s="65"/>
+      <c r="U10" s="66">
+        <v>46</v>
+      </c>
+      <c r="V10" s="66">
+        <v>47</v>
+      </c>
+      <c r="W10" s="65"/>
+      <c r="X10" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="67">
+        <v>161</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="39"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="66">
+        <v>48</v>
+      </c>
+      <c r="D12" s="66">
+        <v>49</v>
+      </c>
+      <c r="E12" s="66">
+        <v>50</v>
+      </c>
+      <c r="F12" s="65"/>
+      <c r="G12" s="66">
+        <v>51</v>
+      </c>
+      <c r="H12" s="66">
+        <v>52</v>
+      </c>
+      <c r="I12" s="66">
+        <v>53</v>
+      </c>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66">
+        <v>54</v>
+      </c>
+      <c r="L12" s="66">
+        <v>55</v>
+      </c>
+      <c r="M12" s="65"/>
+      <c r="N12" s="66">
+        <v>56</v>
+      </c>
+      <c r="O12" s="66">
+        <v>57</v>
+      </c>
+      <c r="P12" s="66">
+        <v>58</v>
+      </c>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="66">
+        <v>59</v>
+      </c>
+      <c r="S12" s="66">
+        <v>60</v>
+      </c>
+      <c r="T12" s="66">
+        <v>61</v>
+      </c>
+      <c r="U12" s="65"/>
+      <c r="V12" s="66">
+        <v>62</v>
+      </c>
+      <c r="W12" s="65"/>
+      <c r="X12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="66">
+        <v>63</v>
+      </c>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="66">
+        <v>64</v>
+      </c>
+      <c r="S13" s="64"/>
+      <c r="T13" s="65"/>
+      <c r="U13" s="64"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="64"/>
+      <c r="X13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66">
+        <v>65</v>
+      </c>
+      <c r="E14" s="66">
+        <v>66</v>
+      </c>
+      <c r="F14" s="66">
+        <v>67</v>
+      </c>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="66">
+        <v>68</v>
+      </c>
+      <c r="K14" s="69"/>
+      <c r="L14" s="70">
+        <v>163</v>
+      </c>
+      <c r="M14" s="71">
+        <v>164</v>
+      </c>
+      <c r="N14" s="72">
+        <v>165</v>
+      </c>
+      <c r="O14" s="73"/>
+      <c r="P14" s="66">
+        <v>69</v>
+      </c>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="64"/>
+      <c r="T14" s="66">
+        <v>70</v>
+      </c>
+      <c r="U14" s="65"/>
+      <c r="V14" s="66">
+        <v>71</v>
+      </c>
+      <c r="W14" s="65"/>
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66">
+        <v>72</v>
+      </c>
+      <c r="E15" s="66">
+        <v>73</v>
+      </c>
+      <c r="F15" s="66">
+        <v>74</v>
+      </c>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66">
+        <v>75</v>
+      </c>
+      <c r="I15" s="65"/>
+      <c r="J15" s="66">
+        <v>76</v>
+      </c>
+      <c r="K15" s="69"/>
+      <c r="L15" s="74">
+        <v>166</v>
+      </c>
+      <c r="M15" s="75">
+        <v>167</v>
+      </c>
+      <c r="N15" s="76">
+        <v>168</v>
+      </c>
+      <c r="O15" s="73"/>
+      <c r="P15" s="66">
+        <v>77</v>
+      </c>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66">
+        <v>78</v>
+      </c>
+      <c r="S15" s="65"/>
+      <c r="T15" s="66">
+        <v>79</v>
+      </c>
+      <c r="U15" s="65"/>
+      <c r="V15" s="66">
+        <v>80</v>
+      </c>
+      <c r="W15" s="65"/>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="66">
+        <v>81</v>
+      </c>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66">
+        <v>82</v>
+      </c>
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="78">
+        <v>169</v>
+      </c>
+      <c r="M16" s="79">
+        <v>170</v>
+      </c>
+      <c r="N16" s="80">
+        <v>171</v>
+      </c>
+      <c r="O16" s="81"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="64"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="64"/>
+      <c r="T16" s="65"/>
+      <c r="U16" s="64"/>
+      <c r="V16" s="66">
+        <v>83</v>
+      </c>
+      <c r="W16" s="65"/>
+      <c r="X16" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>-2</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="66">
+        <v>84</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="66">
+        <v>85</v>
+      </c>
+      <c r="K17" s="64"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="66">
+        <v>86</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>87</v>
+      </c>
+      <c r="R17" s="66">
+        <v>88</v>
+      </c>
+      <c r="S17" s="65"/>
+      <c r="T17" s="66">
+        <v>89</v>
+      </c>
+      <c r="U17" s="64"/>
+      <c r="V17" s="65"/>
+      <c r="W17" s="64"/>
+      <c r="X17" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>-3</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="66">
+        <v>90</v>
+      </c>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66">
+        <v>91</v>
+      </c>
+      <c r="G18" s="66">
+        <v>92</v>
+      </c>
+      <c r="H18" s="66">
+        <v>93</v>
+      </c>
+      <c r="I18" s="65"/>
+      <c r="J18" s="66">
+        <v>94</v>
+      </c>
+      <c r="K18" s="66">
+        <v>95</v>
+      </c>
+      <c r="L18" s="66">
+        <v>96</v>
+      </c>
+      <c r="M18" s="65"/>
+      <c r="N18" s="66">
+        <v>97</v>
+      </c>
+      <c r="O18" s="66">
+        <v>98</v>
+      </c>
+      <c r="P18" s="66">
+        <v>99</v>
+      </c>
+      <c r="Q18" s="64"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="64"/>
+      <c r="T18" s="66">
+        <v>100</v>
+      </c>
+      <c r="U18" s="66">
+        <v>101</v>
+      </c>
+      <c r="V18" s="66">
+        <v>102</v>
+      </c>
+      <c r="W18" s="66">
+        <v>103</v>
+      </c>
+      <c r="X18" s="2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>-4</v>
+      </c>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="66">
+        <v>104</v>
+      </c>
+      <c r="O19" s="66">
+        <v>105</v>
+      </c>
+      <c r="P19" s="66">
+        <v>106</v>
+      </c>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="66">
+        <v>107</v>
+      </c>
+      <c r="S19" s="64"/>
+      <c r="T19" s="65"/>
+      <c r="U19" s="65"/>
+      <c r="V19" s="65"/>
+      <c r="W19" s="67">
+        <v>162</v>
+      </c>
+      <c r="X19" s="2">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>-5</v>
+      </c>
+      <c r="C20" s="66">
+        <v>108</v>
+      </c>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66">
+        <v>109</v>
+      </c>
+      <c r="F20" s="66">
+        <v>110</v>
+      </c>
+      <c r="G20" s="65"/>
+      <c r="H20" s="66">
+        <v>111</v>
+      </c>
+      <c r="I20" s="66">
+        <v>112</v>
+      </c>
+      <c r="J20" s="66">
+        <v>113</v>
+      </c>
+      <c r="K20" s="66">
+        <v>114</v>
+      </c>
+      <c r="L20" s="66">
+        <v>115</v>
+      </c>
+      <c r="M20" s="64"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="64"/>
+      <c r="R20" s="66">
+        <v>116</v>
+      </c>
+      <c r="S20" s="65"/>
+      <c r="T20" s="66">
+        <v>117</v>
+      </c>
+      <c r="U20" s="66">
+        <v>118</v>
+      </c>
+      <c r="V20" s="66">
+        <v>119</v>
+      </c>
+      <c r="W20" s="66">
+        <v>120</v>
+      </c>
+      <c r="X20" s="2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>-6</v>
+      </c>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="66">
+        <v>121</v>
+      </c>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="66">
+        <v>122</v>
+      </c>
+      <c r="O21" s="66">
+        <v>123</v>
+      </c>
+      <c r="P21" s="66">
+        <v>124</v>
+      </c>
+      <c r="Q21" s="64"/>
+      <c r="R21" s="65"/>
+      <c r="S21" s="64"/>
+      <c r="T21" s="65"/>
+      <c r="U21" s="65"/>
+      <c r="V21" s="65"/>
+      <c r="W21" s="64"/>
+      <c r="X21" s="2">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>-7</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66">
+        <v>125</v>
+      </c>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66">
+        <v>126</v>
+      </c>
+      <c r="G22" s="65"/>
+      <c r="H22" s="66">
+        <v>127</v>
+      </c>
+      <c r="I22" s="67">
+        <v>160</v>
+      </c>
+      <c r="J22" s="66">
+        <v>128</v>
+      </c>
+      <c r="K22" s="66">
+        <v>129</v>
+      </c>
+      <c r="L22" s="66">
+        <v>130</v>
+      </c>
+      <c r="M22" s="65"/>
+      <c r="N22" s="66">
+        <v>131</v>
+      </c>
+      <c r="O22" s="64"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="66">
+        <v>132</v>
+      </c>
+      <c r="S22" s="65"/>
+      <c r="T22" s="66">
+        <v>133</v>
+      </c>
+      <c r="U22" s="66">
+        <v>134</v>
+      </c>
+      <c r="V22" s="66">
+        <v>135</v>
+      </c>
+      <c r="W22" s="65"/>
+      <c r="X22" s="2">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>-8</v>
+      </c>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="66">
+        <v>136</v>
+      </c>
+      <c r="I23" s="66">
+        <v>137</v>
+      </c>
+      <c r="J23" s="66">
+        <v>138</v>
+      </c>
+      <c r="K23" s="64"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="66">
+        <v>139</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>140</v>
+      </c>
+      <c r="R23" s="66">
+        <v>141</v>
+      </c>
+      <c r="S23" s="64"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="65"/>
+      <c r="W23" s="64"/>
+      <c r="X23" s="2">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <v>-9</v>
+      </c>
+      <c r="C24" s="65"/>
+      <c r="D24" s="66">
+        <v>142</v>
+      </c>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66">
+        <v>143</v>
+      </c>
+      <c r="G24" s="65"/>
+      <c r="H24" s="66">
+        <v>144</v>
+      </c>
+      <c r="I24" s="66">
+        <v>145</v>
+      </c>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="66">
+        <v>146</v>
+      </c>
+      <c r="M24" s="66">
+        <v>147</v>
+      </c>
+      <c r="N24" s="66">
+        <v>148</v>
+      </c>
+      <c r="O24" s="64"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="66">
+        <v>149</v>
+      </c>
+      <c r="S24" s="65"/>
+      <c r="T24" s="66">
+        <v>150</v>
+      </c>
+      <c r="U24" s="66">
+        <v>151</v>
+      </c>
+      <c r="V24" s="66">
+        <v>152</v>
+      </c>
+      <c r="W24" s="65"/>
+      <c r="X24" s="2">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>-10</v>
+      </c>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="66">
+        <v>153</v>
+      </c>
+      <c r="L25" s="66">
+        <v>154</v>
+      </c>
+      <c r="M25" s="66">
+        <v>155</v>
+      </c>
+      <c r="N25" s="66">
+        <v>156</v>
+      </c>
+      <c r="O25" s="66">
+        <v>157</v>
+      </c>
+      <c r="P25" s="66">
+        <v>158</v>
+      </c>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="64"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="64"/>
+      <c r="X25" s="2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="4">
+        <v>-10</v>
+      </c>
+      <c r="D26" s="4">
+        <v>-9</v>
+      </c>
+      <c r="E26" s="4">
+        <v>-8</v>
+      </c>
+      <c r="F26" s="4">
+        <v>-7</v>
+      </c>
+      <c r="G26" s="4">
+        <v>-6</v>
+      </c>
+      <c r="H26" s="4">
+        <v>-5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>-4</v>
+      </c>
+      <c r="J26" s="4">
+        <v>-3</v>
+      </c>
+      <c r="K26" s="4">
+        <v>-2</v>
+      </c>
+      <c r="L26" s="4">
+        <v>-1</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2</v>
+      </c>
+      <c r="P26" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>4</v>
+      </c>
+      <c r="R26" s="4">
+        <v>5</v>
+      </c>
+      <c r="S26" s="4">
+        <v>6</v>
+      </c>
+      <c r="T26" s="4">
+        <v>7</v>
+      </c>
+      <c r="U26" s="4">
+        <v>8</v>
+      </c>
+      <c r="V26" s="4">
+        <v>9</v>
+      </c>
+      <c r="W26" s="4">
+        <v>10</v>
+      </c>
+      <c r="X26" s="19"/>
+    </row>
+    <row r="27" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:X2"/>
+    <mergeCell ref="Z6:AA6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07115DE1-BD17-4EFB-B602-D356C0068EC1}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -3756,76 +5049,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="66"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+      <c r="AA1" s="85"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="85"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="85"/>
+      <c r="AH1" s="86"/>
     </row>
     <row r="2" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="68"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="68"/>
-      <c r="AH2" s="69"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+      <c r="AG2" s="88"/>
+      <c r="AH2" s="89"/>
     </row>
     <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -4076,10 +5369,10 @@
       <c r="AH7" s="2">
         <v>13</v>
       </c>
-      <c r="AJ7" s="70" t="s">
+      <c r="AJ7" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="AK7" s="70"/>
+      <c r="AK7" s="90"/>
     </row>
     <row r="8" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
@@ -5443,7 +6736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF51CC72-5A0D-44FD-BDF2-656FCDA521BB}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -5486,76 +6779,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="66"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+      <c r="AA1" s="85"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="85"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="85"/>
+      <c r="AH1" s="86"/>
     </row>
     <row r="2" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-      <c r="X2" s="68"/>
-      <c r="Y2" s="68"/>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
-      <c r="AE2" s="68"/>
-      <c r="AF2" s="68"/>
-      <c r="AG2" s="68"/>
-      <c r="AH2" s="69"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+      <c r="AG2" s="88"/>
+      <c r="AH2" s="89"/>
     </row>
     <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -5853,10 +7146,10 @@
       <c r="AH7" s="2">
         <v>13</v>
       </c>
-      <c r="AJ7" s="70" t="s">
+      <c r="AJ7" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="AK7" s="70"/>
+      <c r="AK7" s="90"/>
     </row>
     <row r="8" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">

</xml_diff>

<commit_message>
Save slight changes in the Game Level Designs
</commit_message>
<xml_diff>
--- a/Game Level Designs.xlsx
+++ b/Game Level Designs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16EAD4E-863F-42C1-8614-D51CB17D69B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068FB207-8050-4FA4-A76A-CD265A58C4E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645" tabRatio="749" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12645" tabRatio="749" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Level 1" sheetId="3" r:id="rId1"/>
@@ -2637,20 +2637,21 @@
   </sheetPr>
   <dimension ref="B1:AA27"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="2.28515625" bestFit="1" customWidth="1"/>
@@ -2659,7 +2660,7 @@
     <col min="18" max="18" width="1.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.85546875" customWidth="1"/>
     <col min="26" max="26" width="1.42578125" bestFit="1" customWidth="1"/>
@@ -3788,7 +3789,7 @@
   </sheetPr>
   <dimension ref="B1:AA27"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>